<commit_message>
bergupdate: advanced onreport and changed script for comparing GIs
</commit_message>
<xml_diff>
--- a/results/GI_all_methods/gi_results_all_methods.xlsx
+++ b/results/GI_all_methods/gi_results_all_methods.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>sample</t>
   </si>
@@ -175,10 +175,16 @@
     <t>GI Agilent</t>
   </si>
   <si>
-    <t>15 ou 22,5</t>
-  </si>
-  <si>
-    <t>13,5 ou 8,16</t>
+    <t>GI_Agilent</t>
+  </si>
+  <si>
+    <t>GI_Agilent_alternatif</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -2352,13 +2358,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F21"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2377,7 +2386,10 @@
         <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2396,14 +2408,14 @@
       <c r="E2" s="2">
         <v>24.0833333333333</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2">
+      <c r="F2">
         <v>9.14</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2419,11 +2431,11 @@
       <c r="E3" s="16">
         <v>84.375</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>22.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2442,11 +2454,11 @@
       <c r="E4" s="2">
         <v>36.1</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4">
+      <c r="F4">
         <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2465,11 +2477,11 @@
       <c r="E5" s="2">
         <v>36.75</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5">
+      <c r="F5">
         <v>9.1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2488,11 +2500,11 @@
       <c r="E6" s="2">
         <v>60.75</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6">
+      <c r="F6">
         <v>20.6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2511,11 +2523,11 @@
       <c r="E7" s="2">
         <v>23.1428571428571</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7">
+      <c r="F7">
         <v>24.1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2534,11 +2546,11 @@
       <c r="E8" s="2">
         <v>18</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8">
+      <c r="F8">
         <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2557,11 +2569,11 @@
       <c r="E9" s="2">
         <v>6</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9">
+      <c r="F9">
         <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2580,11 +2592,11 @@
       <c r="E10" s="2">
         <v>12.5</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10">
+      <c r="F10">
         <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2603,11 +2615,11 @@
       <c r="E11" s="2">
         <v>36.75</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11">
+      <c r="F11">
         <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2626,11 +2638,11 @@
       <c r="E12" s="2">
         <v>45.125</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12">
+      <c r="F12">
         <v>39.200000000000003</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2649,11 +2661,11 @@
       <c r="E13" s="16">
         <v>96.1</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13">
+      <c r="F13">
         <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2672,11 +2684,11 @@
       <c r="E14" s="2">
         <v>15.363636363636401</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14">
+      <c r="F14">
         <v>9.14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2695,11 +2707,11 @@
       <c r="E15" s="2">
         <v>24.066666666666698</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15">
+      <c r="F15">
         <v>10.6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2718,11 +2730,11 @@
       <c r="E16" s="2">
         <v>16.899999999999999</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16">
+      <c r="F16">
         <v>10.6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2741,14 +2753,14 @@
       <c r="E17" s="16">
         <v>416.89473684210498</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17">
+      <c r="F17">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -2764,14 +2776,14 @@
       <c r="E18" s="2">
         <v>23.272727272727298</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>13.5</v>
+      </c>
+      <c r="G18">
+        <v>8.16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
@@ -2787,14 +2799,14 @@
       <c r="E19" s="2">
         <v>44.307692307692299</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19">
+      <c r="F19">
         <v>9.14</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -2810,14 +2822,14 @@
       <c r="E20" s="2">
         <v>12.1</v>
       </c>
-      <c r="F20" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20">
+      <c r="F20">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -2833,11 +2845,16 @@
       <c r="E21" s="2">
         <v>8.1666666666666696</v>
       </c>
-      <c r="F21" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21">
+      <c r="F21">
         <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bergupdate: Cleaned up ASCAT.R and partially CGHcall.R. Now they produce results cleanlier
</commit_message>
<xml_diff>
--- a/results/GI_all_methods/gi_results_all_methods.xlsx
+++ b/results/GI_all_methods/gi_results_all_methods.xlsx
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="gi_results_all_methods" sheetId="1" r:id="rId1"/>
-    <sheet name="to_export" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="3" r:id="rId2"/>
+    <sheet name="to_export" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="128">
   <si>
     <t>sample</t>
   </si>
@@ -185,6 +186,225 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>NbalterASCAT</t>
+  </si>
+  <si>
+    <t>NbchrASCAT</t>
+  </si>
+  <si>
+    <t>RuntimeASCAT</t>
+  </si>
+  <si>
+    <t>13.44</t>
+  </si>
+  <si>
+    <t>18.78</t>
+  </si>
+  <si>
+    <t>28.13</t>
+  </si>
+  <si>
+    <t>23.2727272727273</t>
+  </si>
+  <si>
+    <t>9.14</t>
+  </si>
+  <si>
+    <t>37.0829110145569</t>
+  </si>
+  <si>
+    <t>26.27</t>
+  </si>
+  <si>
+    <t>19.6</t>
+  </si>
+  <si>
+    <t>36.36</t>
+  </si>
+  <si>
+    <t>69.1363636363636</t>
+  </si>
+  <si>
+    <t>22.5</t>
+  </si>
+  <si>
+    <t>31.5028810501099</t>
+  </si>
+  <si>
+    <t>11.57</t>
+  </si>
+  <si>
+    <t>8.17</t>
+  </si>
+  <si>
+    <t>10.125</t>
+  </si>
+  <si>
+    <t>38.3915300369263</t>
+  </si>
+  <si>
+    <t>25.6</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>39.0917129516602</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>53.78</t>
+  </si>
+  <si>
+    <t>62.5</t>
+  </si>
+  <si>
+    <t>20.6</t>
+  </si>
+  <si>
+    <t>38.1577680110931</t>
+  </si>
+  <si>
+    <t>24.14</t>
+  </si>
+  <si>
+    <t>17.82</t>
+  </si>
+  <si>
+    <t>21.3333333333333</t>
+  </si>
+  <si>
+    <t>24.1</t>
+  </si>
+  <si>
+    <t>35.3019709587097</t>
+  </si>
+  <si>
+    <t>6.25</t>
+  </si>
+  <si>
+    <t>13.5</t>
+  </si>
+  <si>
+    <t>37.3849618434906</t>
+  </si>
+  <si>
+    <t>10.67</t>
+  </si>
+  <si>
+    <t>39.1437752246857</t>
+  </si>
+  <si>
+    <t>9.14285714285714</t>
+  </si>
+  <si>
+    <t>37.1163249015808</t>
+  </si>
+  <si>
+    <t>75.11</t>
+  </si>
+  <si>
+    <t>32.4</t>
+  </si>
+  <si>
+    <t>39.6746289730072</t>
+  </si>
+  <si>
+    <t>46.2857142857143</t>
+  </si>
+  <si>
+    <t>39.2</t>
+  </si>
+  <si>
+    <t>32.778088092804</t>
+  </si>
+  <si>
+    <t>82.29</t>
+  </si>
+  <si>
+    <t>80.67</t>
+  </si>
+  <si>
+    <t>105.125</t>
+  </si>
+  <si>
+    <t>38.2369520664215</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>13.4444444444444</t>
+  </si>
+  <si>
+    <t>34.1809649467468</t>
+  </si>
+  <si>
+    <t>22.2307692307692</t>
+  </si>
+  <si>
+    <t>10.6</t>
+  </si>
+  <si>
+    <t>32.6668920516968</t>
+  </si>
+  <si>
+    <t>14.29</t>
+  </si>
+  <si>
+    <t>16.67</t>
+  </si>
+  <si>
+    <t>15.125</t>
+  </si>
+  <si>
+    <t>33.4308669567108</t>
+  </si>
+  <si>
+    <t>8.33</t>
+  </si>
+  <si>
+    <t>395.529411764706</t>
+  </si>
+  <si>
+    <t>12.8</t>
+  </si>
+  <si>
+    <t>33.0491781234741</t>
+  </si>
+  <si>
+    <t>21.7777777777778</t>
+  </si>
+  <si>
+    <t>8.16</t>
+  </si>
+  <si>
+    <t>38.7418110370636</t>
+  </si>
+  <si>
+    <t>44.0833333333333</t>
+  </si>
+  <si>
+    <t>34.6241869926453</t>
+  </si>
+  <si>
+    <t>21.13</t>
+  </si>
+  <si>
+    <t>40.5704288482666</t>
+  </si>
+  <si>
+    <t>20.17</t>
+  </si>
+  <si>
+    <t>24.2</t>
+  </si>
+  <si>
+    <t>38.1967129707336</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1318,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B21"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,9 +2578,708 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3">
+        <v>39</v>
+      </c>
+      <c r="J3">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5">
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6">
+        <v>25</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>7</v>
+      </c>
+      <c r="K10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11">
+        <v>18</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12">
+        <v>18</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13">
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13">
+        <v>29</v>
+      </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="K13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14">
+        <v>11</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I15">
+        <v>17</v>
+      </c>
+      <c r="J15">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" t="s">
+        <v>112</v>
+      </c>
+      <c r="I16">
+        <v>11</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+      <c r="K16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17">
+        <v>82</v>
+      </c>
+      <c r="J17">
+        <v>17</v>
+      </c>
+      <c r="K17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18">
+        <v>14</v>
+      </c>
+      <c r="J18">
+        <v>9</v>
+      </c>
+      <c r="K18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" t="s">
+        <v>121</v>
+      </c>
+      <c r="I19">
+        <v>23</v>
+      </c>
+      <c r="J19">
+        <v>12</v>
+      </c>
+      <c r="K19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20">
+        <v>9</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+      <c r="K20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bergupdate: We discussed the results with CL, ED, MA & IS. I added 1-RV sample to scripts. Also I finished Mat & Met
</commit_message>
<xml_diff>
--- a/results/GI_all_methods/gi_results_all_methods.xlsx
+++ b/results/GI_all_methods/gi_results_all_methods.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="gi_results_all_methods" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1" sheetId="3" r:id="rId2"/>
+    <sheet name="old_gi_all_methods" sheetId="1" r:id="rId1"/>
+    <sheet name="new_gi_all_methods" sheetId="3" r:id="rId2"/>
     <sheet name="to_export" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
   <si>
     <t>sample</t>
   </si>
@@ -188,223 +188,31 @@
     <t>S</t>
   </si>
   <si>
-    <t>NbalterASCAT</t>
-  </si>
-  <si>
-    <t>NbchrASCAT</t>
-  </si>
-  <si>
-    <t>RuntimeASCAT</t>
-  </si>
-  <si>
-    <t>13.44</t>
-  </si>
-  <si>
-    <t>18.78</t>
-  </si>
-  <si>
-    <t>28.13</t>
-  </si>
-  <si>
-    <t>23.2727272727273</t>
-  </si>
-  <si>
-    <t>9.14</t>
-  </si>
-  <si>
-    <t>37.0829110145569</t>
-  </si>
-  <si>
-    <t>26.27</t>
-  </si>
-  <si>
-    <t>19.6</t>
-  </si>
-  <si>
-    <t>36.36</t>
-  </si>
-  <si>
-    <t>69.1363636363636</t>
-  </si>
-  <si>
-    <t>22.5</t>
-  </si>
-  <si>
-    <t>31.5028810501099</t>
-  </si>
-  <si>
-    <t>11.57</t>
-  </si>
-  <si>
-    <t>8.17</t>
-  </si>
-  <si>
-    <t>10.125</t>
-  </si>
-  <si>
-    <t>38.3915300369263</t>
-  </si>
-  <si>
-    <t>25.6</t>
-  </si>
-  <si>
-    <t>9.1</t>
-  </si>
-  <si>
-    <t>39.0917129516602</t>
-  </si>
-  <si>
-    <t>7.2</t>
-  </si>
-  <si>
-    <t>53.78</t>
-  </si>
-  <si>
-    <t>62.5</t>
-  </si>
-  <si>
-    <t>20.6</t>
-  </si>
-  <si>
-    <t>38.1577680110931</t>
-  </si>
-  <si>
-    <t>24.14</t>
-  </si>
-  <si>
-    <t>17.82</t>
-  </si>
-  <si>
-    <t>21.3333333333333</t>
-  </si>
-  <si>
-    <t>24.1</t>
-  </si>
-  <si>
-    <t>35.3019709587097</t>
-  </si>
-  <si>
-    <t>6.25</t>
-  </si>
-  <si>
-    <t>13.5</t>
-  </si>
-  <si>
-    <t>37.3849618434906</t>
-  </si>
-  <si>
-    <t>10.67</t>
-  </si>
-  <si>
-    <t>39.1437752246857</t>
-  </si>
-  <si>
-    <t>9.14285714285714</t>
-  </si>
-  <si>
-    <t>37.1163249015808</t>
-  </si>
-  <si>
-    <t>75.11</t>
-  </si>
-  <si>
-    <t>32.4</t>
-  </si>
-  <si>
-    <t>39.6746289730072</t>
-  </si>
-  <si>
-    <t>46.2857142857143</t>
-  </si>
-  <si>
-    <t>39.2</t>
-  </si>
-  <si>
-    <t>32.778088092804</t>
-  </si>
-  <si>
-    <t>82.29</t>
-  </si>
-  <si>
-    <t>80.67</t>
-  </si>
-  <si>
-    <t>105.125</t>
-  </si>
-  <si>
-    <t>38.2369520664215</t>
-  </si>
-  <si>
-    <t>12.5</t>
-  </si>
-  <si>
-    <t>13.4444444444444</t>
-  </si>
-  <si>
-    <t>34.1809649467468</t>
-  </si>
-  <si>
-    <t>22.2307692307692</t>
-  </si>
-  <si>
-    <t>10.6</t>
-  </si>
-  <si>
-    <t>32.6668920516968</t>
-  </si>
-  <si>
-    <t>14.29</t>
-  </si>
-  <si>
-    <t>16.67</t>
-  </si>
-  <si>
-    <t>15.125</t>
-  </si>
-  <si>
-    <t>33.4308669567108</t>
-  </si>
-  <si>
-    <t>8.33</t>
-  </si>
-  <si>
-    <t>395.529411764706</t>
-  </si>
-  <si>
-    <t>12.8</t>
-  </si>
-  <si>
-    <t>33.0491781234741</t>
-  </si>
-  <si>
-    <t>21.7777777777778</t>
-  </si>
-  <si>
-    <t>8.16</t>
-  </si>
-  <si>
-    <t>38.7418110370636</t>
-  </si>
-  <si>
-    <t>44.0833333333333</t>
-  </si>
-  <si>
-    <t>34.6241869926453</t>
-  </si>
-  <si>
-    <t>21.13</t>
-  </si>
-  <si>
-    <t>40.5704288482666</t>
-  </si>
-  <si>
-    <t>20.17</t>
-  </si>
-  <si>
-    <t>24.2</t>
-  </si>
-  <si>
-    <t>38.1967129707336</t>
+    <t>nbAlter_ASCAT</t>
+  </si>
+  <si>
+    <t>nbChr_ASCAT</t>
+  </si>
+  <si>
+    <t>runTime_ASCAT</t>
+  </si>
+  <si>
+    <t>estimPurity_ASCAT</t>
+  </si>
+  <si>
+    <t>purity_HES</t>
+  </si>
+  <si>
+    <t>runTime_CGHcall</t>
+  </si>
+  <si>
+    <t>runTime_rCGH</t>
+  </si>
+  <si>
+    <t>runTime_oncoscanR</t>
+  </si>
+  <si>
+    <t>1-RV</t>
   </si>
 </sst>
 </file>
@@ -555,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -777,8 +585,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -908,6 +722,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -953,7 +780,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -985,6 +812,14 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1315,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,108 +1220,97 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17">
+        <v>1</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17">
+        <v>1</v>
+      </c>
+      <c r="G2" s="17">
+        <v>1</v>
+      </c>
+      <c r="H2" s="17">
+        <v>1</v>
+      </c>
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="17">
+        <v>1</v>
+      </c>
+      <c r="K2" s="17">
+        <v>1</v>
+      </c>
+      <c r="L2" s="17">
+        <v>1</v>
+      </c>
+      <c r="M2" s="17">
+        <v>1</v>
+      </c>
+      <c r="N2" s="17">
+        <v>1</v>
+      </c>
+      <c r="O2" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="5">
         <v>13.4444444444444</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D3" s="6">
         <v>11</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E3" s="6">
         <v>9</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F3" s="7">
         <v>18.7777777777778</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G3" s="8">
         <v>13</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H3" s="8">
         <v>9</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I3" s="9">
         <v>28.125</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J3" s="10">
         <v>15</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K3" s="10">
         <v>8</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L3" s="2">
         <v>24.0833333333333</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M3" s="11">
         <v>17</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N3" s="11">
         <v>12</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O3" s="2">
         <v>34.061813116073601</v>
-      </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="5">
-        <v>26.272727272727298</v>
-      </c>
-      <c r="D3" s="6">
-        <v>17</v>
-      </c>
-      <c r="E3" s="6">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="G3" s="8">
-        <v>14</v>
-      </c>
-      <c r="H3" s="8">
-        <v>10</v>
-      </c>
-      <c r="I3" s="9">
-        <v>36.363636363636402</v>
-      </c>
-      <c r="J3" s="10">
-        <v>20</v>
-      </c>
-      <c r="K3" s="10">
-        <v>11</v>
-      </c>
-      <c r="L3" s="16">
-        <v>84.375</v>
-      </c>
-      <c r="M3" s="11">
-        <v>45</v>
-      </c>
-      <c r="N3" s="11">
-        <v>24</v>
-      </c>
-      <c r="O3" s="2">
-        <v>29.838351964950601</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1500,51 +1324,51 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>28</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C4" s="5">
-        <v>4</v>
+        <v>26.272727272727298</v>
       </c>
       <c r="D4" s="6">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E4" s="6">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F4" s="7">
-        <v>11.5714285714286</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="G4" s="8">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H4" s="8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I4" s="9">
-        <v>8.1666666666666696</v>
+        <v>36.363636363636402</v>
       </c>
       <c r="J4" s="10">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="K4" s="10">
-        <v>6</v>
-      </c>
-      <c r="L4" s="2">
-        <v>36.1</v>
+        <v>11</v>
+      </c>
+      <c r="L4" s="16">
+        <v>84.375</v>
       </c>
       <c r="M4" s="11">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="N4" s="11">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="O4" s="2">
-        <v>37.573472023010297</v>
+        <v>29.838351964950601</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -1560,49 +1384,49 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C5" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="7">
-        <v>18.7777777777778</v>
+        <v>11.5714285714286</v>
       </c>
       <c r="G5" s="8">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H5" s="8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I5" s="9">
-        <v>32</v>
+        <v>8.1666666666666696</v>
       </c>
       <c r="J5" s="10">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="K5" s="10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L5" s="2">
-        <v>36.75</v>
+        <v>36.1</v>
       </c>
       <c r="M5" s="11">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N5" s="11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O5" s="2">
-        <v>38.198194980621302</v>
+        <v>37.573472023010297</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -1618,49 +1442,49 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="5">
-        <v>7.2</v>
+        <v>5</v>
       </c>
       <c r="D6" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="6">
         <v>5</v>
       </c>
       <c r="F6" s="7">
-        <v>53.7777777777778</v>
+        <v>18.7777777777778</v>
       </c>
       <c r="G6" s="8">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H6" s="8">
         <v>9</v>
       </c>
       <c r="I6" s="9">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="J6" s="10">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K6" s="10">
         <v>8</v>
       </c>
       <c r="L6" s="2">
-        <v>60.75</v>
+        <v>36.75</v>
       </c>
       <c r="M6" s="11">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="N6" s="11">
         <v>12</v>
       </c>
       <c r="O6" s="2">
-        <v>36.393515110015898</v>
+        <v>38.198194980621302</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1676,49 +1500,49 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="5">
-        <v>24.1428571428571</v>
+        <v>7.2</v>
       </c>
       <c r="D7" s="6">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E7" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7" s="7">
-        <v>17.818181818181799</v>
+        <v>53.7777777777778</v>
       </c>
       <c r="G7" s="8">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H7" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I7" s="9">
-        <v>19.600000000000001</v>
+        <v>50</v>
       </c>
       <c r="J7" s="10">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="K7" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L7" s="2">
-        <v>23.1428571428571</v>
+        <v>60.75</v>
       </c>
       <c r="M7" s="11">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="N7" s="11">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O7" s="2">
-        <v>35.770901918411298</v>
+        <v>36.393515110015898</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1734,49 +1558,49 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>29</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="C8" s="5">
-        <v>1</v>
+        <v>24.1428571428571</v>
       </c>
       <c r="D8" s="6">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E8" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F8" s="7">
-        <v>6.25</v>
+        <v>17.818181818181799</v>
       </c>
       <c r="G8" s="8">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H8" s="8">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I8" s="9">
-        <v>2</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="J8" s="10">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K8" s="10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L8" s="2">
+        <v>23.1428571428571</v>
+      </c>
+      <c r="M8" s="11">
         <v>18</v>
       </c>
-      <c r="M8" s="11">
-        <v>12</v>
-      </c>
       <c r="N8" s="11">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="O8" s="2">
-        <v>38.241448879241901</v>
+        <v>35.770901918411298</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -1792,49 +1616,49 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>6.25</v>
+      </c>
+      <c r="G9" s="8">
+        <v>5</v>
+      </c>
+      <c r="H9" s="8">
+        <v>4</v>
+      </c>
+      <c r="I9" s="9">
         <v>2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="J9" s="10">
         <v>2</v>
       </c>
-      <c r="E9" s="6">
+      <c r="K9" s="10">
         <v>2</v>
       </c>
-      <c r="F9" s="7">
-        <v>10.6666666666667</v>
-      </c>
-      <c r="G9" s="8">
+      <c r="L9" s="2">
+        <v>18</v>
+      </c>
+      <c r="M9" s="11">
+        <v>12</v>
+      </c>
+      <c r="N9" s="11">
         <v>8</v>
       </c>
-      <c r="H9" s="8">
-        <v>6</v>
-      </c>
-      <c r="I9" s="9">
-        <v>1</v>
-      </c>
-      <c r="J9" s="10">
-        <v>1</v>
-      </c>
-      <c r="K9" s="10">
-        <v>1</v>
-      </c>
-      <c r="L9" s="2">
-        <v>6</v>
-      </c>
-      <c r="M9" s="11">
-        <v>6</v>
-      </c>
-      <c r="N9" s="11">
-        <v>6</v>
-      </c>
       <c r="O9" s="2">
-        <v>39.847757101059003</v>
+        <v>38.241448879241901</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1850,10 +1674,10 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
@@ -1865,34 +1689,34 @@
         <v>2</v>
       </c>
       <c r="F10" s="7">
-        <v>11.5714285714286</v>
+        <v>10.6666666666667</v>
       </c>
       <c r="G10" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I10" s="9">
-        <v>13.5</v>
+        <v>1</v>
       </c>
       <c r="J10" s="10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K10" s="10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
         <v>6</v>
       </c>
-      <c r="L10" s="2">
-        <v>12.5</v>
-      </c>
       <c r="M10" s="11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="N10" s="11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O10" s="2">
-        <v>36.7508769035339</v>
+        <v>39.847757101059003</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -1908,49 +1732,49 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D11" s="6">
+        <v>2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>11.5714285714286</v>
+      </c>
+      <c r="G11" s="8">
+        <v>9</v>
+      </c>
+      <c r="H11" s="8">
+        <v>7</v>
+      </c>
+      <c r="I11" s="9">
+        <v>13.5</v>
+      </c>
+      <c r="J11" s="10">
+        <v>9</v>
+      </c>
+      <c r="K11" s="10">
         <v>6</v>
       </c>
-      <c r="E11" s="6">
-        <v>3</v>
-      </c>
-      <c r="F11" s="7">
-        <v>36</v>
-      </c>
-      <c r="G11" s="8">
-        <v>18</v>
-      </c>
-      <c r="H11" s="8">
-        <v>9</v>
-      </c>
-      <c r="I11" s="16">
-        <v>75.1111111111111</v>
-      </c>
-      <c r="J11" s="10">
-        <v>26</v>
-      </c>
-      <c r="K11" s="10">
-        <v>9</v>
-      </c>
       <c r="L11" s="2">
-        <v>36.75</v>
+        <v>12.5</v>
       </c>
       <c r="M11" s="11">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N11" s="11">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O11" s="2">
-        <v>39.109652996063197</v>
+        <v>36.7508769035339</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -1966,49 +1790,49 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="5">
         <v>12</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
       <c r="D12" s="6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E12" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="7">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="G12" s="8">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H12" s="8">
-        <v>8</v>
-      </c>
-      <c r="I12" s="9">
-        <v>53.7777777777778</v>
+        <v>9</v>
+      </c>
+      <c r="I12" s="16">
+        <v>75.1111111111111</v>
       </c>
       <c r="J12" s="10">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K12" s="10">
         <v>9</v>
       </c>
       <c r="L12" s="2">
-        <v>45.125</v>
+        <v>36.75</v>
       </c>
       <c r="M12" s="11">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N12" s="11">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O12" s="2">
-        <v>31.3841421604156</v>
+        <v>39.109652996063197</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -2024,49 +1848,49 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5">
-        <v>6.25</v>
+        <v>0</v>
       </c>
       <c r="D13" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E13" s="6">
-        <v>4</v>
-      </c>
-      <c r="F13" s="16">
-        <v>82.285714285714306</v>
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>72</v>
       </c>
       <c r="G13" s="8">
         <v>24</v>
       </c>
       <c r="H13" s="8">
-        <v>7</v>
-      </c>
-      <c r="I13" s="16">
-        <v>80.6666666666667</v>
+        <v>8</v>
+      </c>
+      <c r="I13" s="9">
+        <v>53.7777777777778</v>
       </c>
       <c r="J13" s="10">
         <v>22</v>
       </c>
       <c r="K13" s="10">
-        <v>6</v>
-      </c>
-      <c r="L13" s="16">
-        <v>96.1</v>
+        <v>9</v>
+      </c>
+      <c r="L13" s="2">
+        <v>45.125</v>
       </c>
       <c r="M13" s="11">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="N13" s="11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O13" s="2">
-        <v>37.831223964691198</v>
+        <v>31.3841421604156</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -2082,49 +1906,49 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>37</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C14" s="5">
-        <v>13.4444444444444</v>
+        <v>6.25</v>
       </c>
       <c r="D14" s="6">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E14" s="6">
-        <v>9</v>
-      </c>
-      <c r="F14" s="7">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F14" s="16">
+        <v>82.285714285714306</v>
       </c>
       <c r="G14" s="8">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H14" s="8">
-        <v>8</v>
-      </c>
-      <c r="I14" s="9">
-        <v>12.5</v>
+        <v>7</v>
+      </c>
+      <c r="I14" s="16">
+        <v>80.6666666666667</v>
       </c>
       <c r="J14" s="10">
+        <v>22</v>
+      </c>
+      <c r="K14" s="10">
+        <v>6</v>
+      </c>
+      <c r="L14" s="16">
+        <v>96.1</v>
+      </c>
+      <c r="M14" s="11">
+        <v>31</v>
+      </c>
+      <c r="N14" s="11">
         <v>10</v>
       </c>
-      <c r="K14" s="10">
-        <v>8</v>
-      </c>
-      <c r="L14" s="2">
-        <v>15.363636363636401</v>
-      </c>
-      <c r="M14" s="11">
-        <v>13</v>
-      </c>
-      <c r="N14" s="11">
-        <v>11</v>
-      </c>
       <c r="O14" s="2">
-        <v>37.461024999618502</v>
+        <v>37.831223964691198</v>
       </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -2140,49 +1964,49 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>43</v>
+        <v>14</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="C15" s="5">
-        <v>10.6666666666667</v>
+        <v>13.4444444444444</v>
       </c>
       <c r="D15" s="6">
+        <v>11</v>
+      </c>
+      <c r="E15" s="6">
+        <v>9</v>
+      </c>
+      <c r="F15" s="7">
         <v>8</v>
       </c>
-      <c r="E15" s="6">
-        <v>6</v>
-      </c>
-      <c r="F15" s="7">
-        <v>24.1428571428571</v>
-      </c>
       <c r="G15" s="8">
+        <v>8</v>
+      </c>
+      <c r="H15" s="8">
+        <v>8</v>
+      </c>
+      <c r="I15" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="J15" s="10">
+        <v>10</v>
+      </c>
+      <c r="K15" s="10">
+        <v>8</v>
+      </c>
+      <c r="L15" s="2">
+        <v>15.363636363636401</v>
+      </c>
+      <c r="M15" s="11">
         <v>13</v>
       </c>
-      <c r="H15" s="8">
-        <v>7</v>
-      </c>
-      <c r="I15" s="9">
-        <v>7.2</v>
-      </c>
-      <c r="J15" s="10">
-        <v>6</v>
-      </c>
-      <c r="K15" s="10">
-        <v>5</v>
-      </c>
-      <c r="L15" s="2">
-        <v>24.066666666666698</v>
-      </c>
-      <c r="M15" s="11">
-        <v>19</v>
-      </c>
       <c r="N15" s="11">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="O15" s="2">
-        <v>32.708219051361098</v>
+        <v>37.461024999618502</v>
       </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -2198,7 +2022,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>43</v>
@@ -2213,34 +2037,34 @@
         <v>6</v>
       </c>
       <c r="F16" s="7">
-        <v>14.285714285714301</v>
+        <v>24.1428571428571</v>
       </c>
       <c r="G16" s="8">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H16" s="8">
         <v>7</v>
       </c>
       <c r="I16" s="9">
-        <v>16.6666666666667</v>
+        <v>7.2</v>
       </c>
       <c r="J16" s="10">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K16" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L16" s="2">
-        <v>16.899999999999999</v>
+        <v>24.066666666666698</v>
       </c>
       <c r="M16" s="11">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N16" s="11">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="O16" s="2">
-        <v>33.582391977310202</v>
+        <v>32.708219051361098</v>
       </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -2256,49 +2080,49 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="5">
-        <v>8.3333333333333304</v>
+        <v>10.6666666666667</v>
       </c>
       <c r="D17" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E17" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F17" s="7">
-        <v>2</v>
+        <v>14.285714285714301</v>
       </c>
       <c r="G17" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H17" s="8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I17" s="9">
-        <v>1</v>
+        <v>16.6666666666667</v>
       </c>
       <c r="J17" s="10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K17" s="10">
-        <v>1</v>
-      </c>
-      <c r="L17" s="16">
-        <v>416.89473684210498</v>
+        <v>6</v>
+      </c>
+      <c r="L17" s="2">
+        <v>16.899999999999999</v>
       </c>
       <c r="M17" s="11">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="N17" s="11">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="O17" s="2">
-        <v>32.8002960681915</v>
+        <v>33.582391977310202</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -2312,51 +2136,51 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="C18" s="5">
-        <v>4</v>
+        <v>8.3333333333333304</v>
       </c>
       <c r="D18" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" s="7">
-        <v>18.7777777777778</v>
+        <v>2</v>
       </c>
       <c r="G18" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H18" s="8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I18" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J18" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K18" s="10">
-        <v>4</v>
-      </c>
-      <c r="L18" s="2">
-        <v>23.272727272727298</v>
+        <v>1</v>
+      </c>
+      <c r="L18" s="16">
+        <v>416.89473684210498</v>
       </c>
       <c r="M18" s="11">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="N18" s="11">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="O18" s="2">
-        <v>38.677893161773703</v>
+        <v>32.8002960681915</v>
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -2370,30 +2194,30 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C19" s="5">
-        <v>9.1428571428571406</v>
+        <v>4</v>
       </c>
       <c r="D19" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E19" s="6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F19" s="7">
-        <v>10</v>
+        <v>18.7777777777778</v>
       </c>
       <c r="G19" s="8">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H19" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I19" s="9">
         <v>4</v>
@@ -2405,16 +2229,16 @@
         <v>4</v>
       </c>
       <c r="L19" s="2">
-        <v>44.307692307692299</v>
+        <v>23.272727272727298</v>
       </c>
       <c r="M19" s="11">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="N19" s="11">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O19" s="2">
-        <v>31.1437091827393</v>
+        <v>38.677893161773703</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -2430,49 +2254,49 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5">
-        <v>6.25</v>
+        <v>9.1428571428571406</v>
       </c>
       <c r="D20" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E20" s="6">
+        <v>7</v>
+      </c>
+      <c r="F20" s="7">
+        <v>10</v>
+      </c>
+      <c r="G20" s="8">
+        <v>10</v>
+      </c>
+      <c r="H20" s="8">
+        <v>10</v>
+      </c>
+      <c r="I20" s="9">
         <v>4</v>
       </c>
-      <c r="F20" s="7">
-        <v>21.125</v>
-      </c>
-      <c r="G20" s="8">
+      <c r="J20" s="10">
+        <v>4</v>
+      </c>
+      <c r="K20" s="10">
+        <v>4</v>
+      </c>
+      <c r="L20" s="2">
+        <v>44.307692307692299</v>
+      </c>
+      <c r="M20" s="11">
+        <v>24</v>
+      </c>
+      <c r="N20" s="11">
         <v>13</v>
       </c>
-      <c r="H20" s="8">
-        <v>8</v>
-      </c>
-      <c r="I20" s="9">
-        <v>13.5</v>
-      </c>
-      <c r="J20" s="10">
-        <v>9</v>
-      </c>
-      <c r="K20" s="10">
-        <v>6</v>
-      </c>
-      <c r="L20" s="2">
-        <v>12.1</v>
-      </c>
-      <c r="M20" s="11">
-        <v>11</v>
-      </c>
-      <c r="N20" s="11">
-        <v>10</v>
-      </c>
       <c r="O20" s="2">
-        <v>42.5773508548737</v>
+        <v>31.1437091827393</v>
       </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -2488,49 +2312,49 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="C21" s="5">
-        <v>1</v>
+        <v>6.25</v>
       </c>
       <c r="D21" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E21" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F21" s="7">
-        <v>20.1666666666667</v>
+        <v>21.125</v>
       </c>
       <c r="G21" s="8">
+        <v>13</v>
+      </c>
+      <c r="H21" s="8">
+        <v>8</v>
+      </c>
+      <c r="I21" s="9">
+        <v>13.5</v>
+      </c>
+      <c r="J21" s="10">
+        <v>9</v>
+      </c>
+      <c r="K21" s="10">
+        <v>6</v>
+      </c>
+      <c r="L21" s="2">
+        <v>12.1</v>
+      </c>
+      <c r="M21" s="11">
         <v>11</v>
       </c>
-      <c r="H21" s="8">
-        <v>6</v>
-      </c>
-      <c r="I21" s="9">
-        <v>24.2</v>
-      </c>
-      <c r="J21" s="10">
-        <v>11</v>
-      </c>
-      <c r="K21" s="10">
-        <v>5</v>
-      </c>
-      <c r="L21" s="2">
-        <v>8.1666666666666696</v>
-      </c>
-      <c r="M21" s="11">
-        <v>7</v>
-      </c>
       <c r="N21" s="11">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O21" s="2">
-        <v>47.831475019454999</v>
+        <v>42.5773508548737</v>
       </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -2544,20 +2368,52 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+    <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7">
+        <v>20.1666666666667</v>
+      </c>
+      <c r="G22" s="8">
+        <v>11</v>
+      </c>
+      <c r="H22" s="8">
+        <v>6</v>
+      </c>
+      <c r="I22" s="9">
+        <v>24.2</v>
+      </c>
+      <c r="J22" s="10">
+        <v>11</v>
+      </c>
+      <c r="K22" s="10">
+        <v>5</v>
+      </c>
+      <c r="L22" s="2">
+        <v>8.1666666666666696</v>
+      </c>
+      <c r="M22" s="11">
+        <v>7</v>
+      </c>
+      <c r="N22" s="11">
+        <v>6</v>
+      </c>
+      <c r="O22" s="2">
+        <v>47.831475019454999</v>
+      </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -2570,6 +2426,32 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2578,27 +2460,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2611,6 +2503,9 @@
       <c r="D1" t="s">
         <v>47</v>
       </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
       <c r="F1" t="s">
         <v>51</v>
       </c>
@@ -2618,656 +2513,1346 @@
         <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="B2" s="5">
+        <v>13.4444444444444</v>
+      </c>
+      <c r="C2" s="7">
+        <v>18.7777777777778</v>
+      </c>
+      <c r="D2" s="9">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>23.272727272727298</v>
+      </c>
+      <c r="F2" s="4">
+        <v>9.14</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2">
+      <c r="H2" s="21">
         <v>16</v>
       </c>
-      <c r="J2">
+      <c r="I2" s="21">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="21">
+        <v>31.9</v>
+      </c>
+      <c r="K2" s="21">
+        <v>0.86</v>
+      </c>
+      <c r="L2" s="21">
+        <v>13</v>
+      </c>
+      <c r="M2" s="21">
+        <v>9</v>
+      </c>
+      <c r="N2" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O2" s="21">
+        <v>7</v>
+      </c>
+      <c r="P2" s="21">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="21">
+        <v>22.13</v>
+      </c>
+      <c r="R2" s="21">
+        <v>11</v>
+      </c>
+      <c r="S2" s="21">
+        <v>9</v>
+      </c>
+      <c r="T2" s="21">
+        <v>9.1310660839080793</v>
+      </c>
+      <c r="U2" s="22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3">
+      <c r="B3" s="5">
+        <v>26.272727272727298</v>
+      </c>
+      <c r="C3" s="7">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="D3" s="9">
+        <v>14.4</v>
+      </c>
+      <c r="E3" s="24">
+        <v>69.136363636363598</v>
+      </c>
+      <c r="F3" s="4">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3">
+      <c r="G3" s="21">
+        <v>22.5</v>
+      </c>
+      <c r="H3" s="21">
         <v>39</v>
       </c>
-      <c r="J3">
+      <c r="I3" s="21">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" s="21">
+        <v>30.52</v>
+      </c>
+      <c r="K3" s="21">
+        <v>0.69</v>
+      </c>
+      <c r="L3" s="21">
+        <v>14</v>
+      </c>
+      <c r="M3" s="21">
+        <v>10</v>
+      </c>
+      <c r="N3" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O3" s="21">
+        <v>12</v>
+      </c>
+      <c r="P3" s="21">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="21">
+        <v>24.36</v>
+      </c>
+      <c r="R3" s="21">
+        <v>17</v>
+      </c>
+      <c r="S3" s="21">
+        <v>11</v>
+      </c>
+      <c r="T3" s="21">
+        <v>21.479266166687001</v>
+      </c>
+      <c r="U3" s="22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4">
+      <c r="C4" s="7">
+        <v>11.5714285714286</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10.125</v>
+      </c>
+      <c r="F4" s="12">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I4">
+      <c r="H4" s="21">
         <v>9</v>
       </c>
-      <c r="J4">
+      <c r="I4" s="21">
         <v>8</v>
       </c>
-      <c r="K4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="21">
+        <v>34.520000000000003</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0.65</v>
+      </c>
+      <c r="L4" s="21">
+        <v>9</v>
+      </c>
+      <c r="M4" s="21">
+        <v>7</v>
+      </c>
+      <c r="N4" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O4" s="21">
+        <v>1</v>
+      </c>
+      <c r="P4" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="21">
+        <v>21.41</v>
+      </c>
+      <c r="R4" s="21">
+        <v>4</v>
+      </c>
+      <c r="S4" s="21">
+        <v>4</v>
+      </c>
+      <c r="T4" s="21">
+        <v>3.2716088294982901</v>
+      </c>
+      <c r="U4" s="23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="C5" s="7">
+        <v>22.5</v>
+      </c>
+      <c r="D5" s="9">
+        <v>16.6666666666667</v>
+      </c>
+      <c r="E5" s="2">
+        <v>25.6</v>
+      </c>
+      <c r="F5" s="12">
+        <v>9.1</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H5" t="s">
-        <v>74</v>
-      </c>
-      <c r="I5">
+      <c r="H5" s="21">
         <v>16</v>
       </c>
-      <c r="J5">
+      <c r="I5" s="21">
         <v>10</v>
       </c>
-      <c r="K5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="21">
+        <v>35.32</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0.83</v>
+      </c>
+      <c r="L5" s="21">
+        <v>15</v>
+      </c>
+      <c r="M5" s="21">
+        <v>10</v>
+      </c>
+      <c r="N5" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O5" s="21">
+        <v>10</v>
+      </c>
+      <c r="P5" s="21">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>25.01</v>
+      </c>
+      <c r="R5" s="21">
+        <v>5</v>
+      </c>
+      <c r="S5" s="21">
+        <v>5</v>
+      </c>
+      <c r="T5" s="21">
+        <v>3.0353591442108199</v>
+      </c>
+      <c r="U5" s="23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="B6" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>53.7777777777778</v>
+      </c>
+      <c r="D6" s="9">
+        <v>36.571428571428598</v>
+      </c>
+      <c r="E6" s="24">
+        <v>62.5</v>
+      </c>
+      <c r="F6" s="12">
+        <v>20.6</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="21">
+        <v>25</v>
+      </c>
+      <c r="I6" s="21">
+        <v>10</v>
+      </c>
+      <c r="J6" s="21">
+        <v>32.76</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0.78</v>
+      </c>
+      <c r="L6" s="21">
+        <v>22</v>
+      </c>
+      <c r="M6" s="21">
+        <v>9</v>
+      </c>
+      <c r="N6" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O6" s="21">
+        <v>16</v>
+      </c>
+      <c r="P6" s="21">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>23.87</v>
+      </c>
+      <c r="R6" s="21">
+        <v>6</v>
+      </c>
+      <c r="S6" s="21">
+        <v>5</v>
+      </c>
+      <c r="T6" s="21">
+        <v>5.2260329723358199</v>
+      </c>
+      <c r="U6" s="23">
         <v>80</v>
       </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6">
-        <v>25</v>
-      </c>
-      <c r="J6">
-        <v>10</v>
-      </c>
-      <c r="K6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="B7" s="5">
+        <v>24.1428571428571</v>
+      </c>
+      <c r="C7" s="7">
+        <v>17.818181818181799</v>
+      </c>
+      <c r="D7" s="9">
+        <v>13.4444444444444</v>
+      </c>
+      <c r="E7" s="2">
+        <v>21.3333333333333</v>
+      </c>
+      <c r="F7" s="12">
+        <v>24.1</v>
+      </c>
+      <c r="G7" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I7">
+      <c r="H7" s="21">
         <v>16</v>
       </c>
-      <c r="J7">
+      <c r="I7" s="21">
         <v>12</v>
       </c>
-      <c r="K7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="21">
+        <v>32.92</v>
+      </c>
+      <c r="K7" s="21">
+        <v>1</v>
+      </c>
+      <c r="L7" s="21">
+        <v>14</v>
+      </c>
+      <c r="M7" s="21">
+        <v>11</v>
+      </c>
+      <c r="N7" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O7" s="21">
+        <v>11</v>
+      </c>
+      <c r="P7" s="21">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>22.93</v>
+      </c>
+      <c r="R7" s="21">
+        <v>13</v>
+      </c>
+      <c r="S7" s="21">
+        <v>7</v>
+      </c>
+      <c r="T7" s="21">
+        <v>6.9933490753173801</v>
+      </c>
+      <c r="U7" s="23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8">
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>6.25</v>
+      </c>
+      <c r="D8" s="9">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>13.5</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="21">
+        <v>9</v>
+      </c>
+      <c r="I8" s="21">
+        <v>6</v>
+      </c>
+      <c r="J8" s="21">
+        <v>36.119999999999997</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0.63</v>
+      </c>
+      <c r="L8" s="21">
+        <v>5</v>
+      </c>
+      <c r="M8" s="21">
+        <v>4</v>
+      </c>
+      <c r="N8" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O8" s="21">
         <v>2</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8">
-        <v>9</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
-      </c>
-      <c r="K8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P8" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>19.079999999999998</v>
+      </c>
+      <c r="R8" s="21">
+        <v>1</v>
+      </c>
+      <c r="S8" s="21">
+        <v>1</v>
+      </c>
+      <c r="T8" s="21">
+        <v>0.52656507492065396</v>
+      </c>
+      <c r="U8" s="22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D9" s="9">
+        <v>8.3333333333333304</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="13">
+        <v>2</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="21">
+        <v>5</v>
+      </c>
+      <c r="I9" s="21">
+        <v>5</v>
+      </c>
+      <c r="J9" s="21">
+        <v>40.26</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0.88</v>
+      </c>
+      <c r="L9" s="21">
+        <v>7</v>
+      </c>
+      <c r="M9" s="21">
+        <v>5</v>
+      </c>
+      <c r="N9" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O9" s="21">
+        <v>5</v>
+      </c>
+      <c r="P9" s="21">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>25.67</v>
+      </c>
+      <c r="R9" s="21">
+        <v>2</v>
+      </c>
+      <c r="S9" s="21">
+        <v>2</v>
+      </c>
+      <c r="T9" s="21">
+        <v>1.3942520618438701</v>
+      </c>
+      <c r="U9" s="22">
         <v>90</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="I9">
-        <v>5</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10">
+      <c r="C10" s="7">
+        <v>11.5714285714286</v>
+      </c>
+      <c r="D10" s="9">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9.1428571428571406</v>
+      </c>
+      <c r="F10" s="13">
         <v>3</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I10">
+      <c r="H10" s="21">
         <v>8</v>
       </c>
-      <c r="J10">
+      <c r="I10" s="21">
         <v>7</v>
       </c>
-      <c r="K10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="21">
+        <v>35.1</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0.89</v>
+      </c>
+      <c r="L10" s="21">
+        <v>9</v>
+      </c>
+      <c r="M10" s="21">
+        <v>7</v>
+      </c>
+      <c r="N10" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O10" s="21">
+        <v>6</v>
+      </c>
+      <c r="P10" s="21">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>20.91</v>
+      </c>
+      <c r="R10" s="21">
+        <v>2</v>
+      </c>
+      <c r="S10" s="21">
+        <v>2</v>
+      </c>
+      <c r="T10" s="21">
+        <v>1.9128990173339799</v>
+      </c>
+      <c r="U10" s="22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="9">
+        <v>24.1428571428571</v>
+      </c>
+      <c r="E11" s="2">
+        <v>32.4</v>
+      </c>
+      <c r="F11" s="13">
         <v>36</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H11" t="s">
-        <v>95</v>
-      </c>
-      <c r="I11">
+      <c r="H11" s="21">
         <v>18</v>
       </c>
-      <c r="J11">
+      <c r="I11" s="21">
         <v>10</v>
       </c>
-      <c r="K11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="21">
+        <v>39.22</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0.82</v>
+      </c>
+      <c r="L11" s="21">
+        <v>18</v>
+      </c>
+      <c r="M11" s="21">
+        <v>9</v>
+      </c>
+      <c r="N11" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O11" s="21">
+        <v>13</v>
+      </c>
+      <c r="P11" s="21">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>23.23</v>
+      </c>
+      <c r="R11" s="21">
+        <v>6</v>
+      </c>
+      <c r="S11" s="21">
+        <v>3</v>
+      </c>
+      <c r="T11" s="21">
+        <v>7.6888940334320104</v>
+      </c>
+      <c r="U11" s="22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="7">
         <v>72</v>
       </c>
-      <c r="D12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="D12" s="9">
+        <v>42.6666666666667</v>
+      </c>
+      <c r="E12" s="2">
+        <v>46.285714285714299</v>
+      </c>
+      <c r="F12" s="13">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H12" t="s">
-        <v>97</v>
-      </c>
-      <c r="I12">
+      <c r="H12" s="21">
         <v>18</v>
       </c>
-      <c r="J12">
+      <c r="I12" s="21">
         <v>7</v>
       </c>
-      <c r="K12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="21">
+        <v>32.549999999999997</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0.86</v>
+      </c>
+      <c r="L12" s="21">
+        <v>24</v>
+      </c>
+      <c r="M12" s="21">
+        <v>8</v>
+      </c>
+      <c r="N12" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O12" s="21">
+        <v>16</v>
+      </c>
+      <c r="P12" s="21">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>25.71</v>
+      </c>
+      <c r="R12" s="21">
+        <v>0</v>
+      </c>
+      <c r="S12" s="21">
+        <v>0</v>
+      </c>
+      <c r="T12" s="21">
+        <v>2.94115114212036</v>
+      </c>
+      <c r="U12" s="22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13">
+      <c r="B13" s="5">
+        <v>6.25</v>
+      </c>
+      <c r="C13" s="24">
+        <v>82.285714285714306</v>
+      </c>
+      <c r="D13" s="24">
+        <v>88.1666666666667</v>
+      </c>
+      <c r="E13" s="24">
+        <v>105.125</v>
+      </c>
+      <c r="F13" s="13">
         <v>60</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H13" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13">
+      <c r="H13" s="21">
         <v>29</v>
       </c>
-      <c r="J13">
+      <c r="I13" s="21">
         <v>8</v>
       </c>
-      <c r="K13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="21">
+        <v>38.31</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0.88</v>
+      </c>
+      <c r="L13" s="21">
+        <v>24</v>
+      </c>
+      <c r="M13" s="21">
+        <v>7</v>
+      </c>
+      <c r="N13" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O13" s="21">
+        <v>23</v>
+      </c>
+      <c r="P13" s="21">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>28.89</v>
+      </c>
+      <c r="R13" s="21">
+        <v>5</v>
+      </c>
+      <c r="S13" s="21">
+        <v>4</v>
+      </c>
+      <c r="T13" s="21">
+        <v>10.073086023330699</v>
+      </c>
+      <c r="U13" s="22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="5">
+        <v>13.4444444444444</v>
+      </c>
+      <c r="C14" s="7">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>13.4444444444444</v>
+      </c>
+      <c r="F14" s="14">
+        <v>9.14</v>
+      </c>
+      <c r="G14" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H14" t="s">
-        <v>105</v>
-      </c>
-      <c r="I14">
+      <c r="H14" s="21">
         <v>11</v>
       </c>
-      <c r="J14">
+      <c r="I14" s="21">
         <v>9</v>
       </c>
-      <c r="K14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="21">
+        <v>36.29</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0.7</v>
+      </c>
+      <c r="L14" s="21">
+        <v>8</v>
+      </c>
+      <c r="M14" s="21">
+        <v>8</v>
+      </c>
+      <c r="N14" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O14" s="21">
+        <v>0</v>
+      </c>
+      <c r="P14" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>27.79</v>
+      </c>
+      <c r="R14" s="21">
+        <v>11</v>
+      </c>
+      <c r="S14" s="21">
+        <v>9</v>
+      </c>
+      <c r="T14" s="21">
+        <v>5.9095079898834202</v>
+      </c>
+      <c r="U14" s="23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" t="s">
-        <v>108</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="B15" s="5">
+        <v>10.6666666666667</v>
+      </c>
+      <c r="C15" s="7">
+        <v>24.1428571428571</v>
+      </c>
+      <c r="D15" s="9">
+        <v>20.1666666666667</v>
+      </c>
+      <c r="E15" s="2">
+        <v>22.230769230769202</v>
+      </c>
+      <c r="F15" s="13">
+        <v>10.6</v>
+      </c>
+      <c r="G15" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H15" t="s">
-        <v>107</v>
-      </c>
-      <c r="I15">
+      <c r="H15" s="21">
         <v>17</v>
       </c>
-      <c r="J15">
+      <c r="I15" s="21">
         <v>13</v>
       </c>
-      <c r="K15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="21">
+        <v>32.53</v>
+      </c>
+      <c r="K15" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="21">
+        <v>13</v>
+      </c>
+      <c r="M15" s="21">
+        <v>7</v>
+      </c>
+      <c r="N15" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O15" s="21">
+        <v>11</v>
+      </c>
+      <c r="P15" s="21">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>40.65</v>
+      </c>
+      <c r="R15" s="21">
+        <v>8</v>
+      </c>
+      <c r="S15" s="21">
+        <v>6</v>
+      </c>
+      <c r="T15" s="21">
+        <v>4.44631099700928</v>
+      </c>
+      <c r="U15" s="22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5">
+        <v>10.6666666666667</v>
+      </c>
+      <c r="C16" s="7">
+        <v>14.285714285714301</v>
+      </c>
+      <c r="D16" s="9">
+        <v>7.2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>15.125</v>
+      </c>
+      <c r="F16" s="13">
+        <v>10.6</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="21">
+        <v>11</v>
+      </c>
+      <c r="I16" s="21">
+        <v>8</v>
+      </c>
+      <c r="J16" s="21">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0.87</v>
+      </c>
+      <c r="L16" s="21">
+        <v>10</v>
+      </c>
+      <c r="M16" s="21">
+        <v>7</v>
+      </c>
+      <c r="N16" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O16" s="21">
+        <v>6</v>
+      </c>
+      <c r="P16" s="21">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>29.47</v>
+      </c>
+      <c r="R16" s="21">
+        <v>8</v>
+      </c>
+      <c r="S16" s="21">
+        <v>6</v>
+      </c>
+      <c r="T16" s="21">
+        <v>7.99450707435608</v>
+      </c>
+      <c r="U16" s="22">
         <v>90</v>
       </c>
-      <c r="C16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" t="s">
-        <v>111</v>
-      </c>
-      <c r="F16" t="s">
-        <v>108</v>
-      </c>
-      <c r="G16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" t="s">
-        <v>112</v>
-      </c>
-      <c r="I16">
-        <v>11</v>
-      </c>
-      <c r="J16">
-        <v>8</v>
-      </c>
-      <c r="K16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="5">
+        <v>8.3333333333333304</v>
+      </c>
+      <c r="C17" s="7">
         <v>2</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="D17" s="9">
+        <v>8.3333333333333304</v>
+      </c>
+      <c r="E17" s="24">
+        <v>395.52941176470603</v>
+      </c>
+      <c r="F17" s="13">
+        <v>12.8</v>
+      </c>
+      <c r="G17" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H17" t="s">
-        <v>115</v>
-      </c>
-      <c r="I17">
+      <c r="H17" s="21">
         <v>82</v>
       </c>
-      <c r="J17">
+      <c r="I17" s="21">
         <v>17</v>
       </c>
-      <c r="K17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="21">
+        <v>34.75</v>
+      </c>
+      <c r="K17" s="21">
+        <v>1</v>
+      </c>
+      <c r="L17" s="21">
+        <v>2</v>
+      </c>
+      <c r="M17" s="21">
+        <v>2</v>
+      </c>
+      <c r="N17" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O17" s="21">
+        <v>5</v>
+      </c>
+      <c r="P17" s="21">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>23.82</v>
+      </c>
+      <c r="R17" s="21">
+        <v>5</v>
+      </c>
+      <c r="S17" s="21">
+        <v>3</v>
+      </c>
+      <c r="T17" s="21">
+        <v>14.0606310367584</v>
+      </c>
+      <c r="U17" s="22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="7">
+        <v>21.7777777777778</v>
+      </c>
+      <c r="D18" s="9">
+        <v>20.1666666666667</v>
+      </c>
+      <c r="E18" s="2">
+        <v>21.7777777777778</v>
+      </c>
+      <c r="F18" s="15">
+        <v>13.5</v>
+      </c>
+      <c r="G18" s="21">
+        <v>8.16</v>
+      </c>
+      <c r="H18" s="21">
+        <v>14</v>
+      </c>
+      <c r="I18" s="21">
+        <v>9</v>
+      </c>
+      <c r="J18" s="21">
+        <v>37.28</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L18" s="21">
+        <v>14</v>
+      </c>
+      <c r="M18" s="21">
+        <v>9</v>
+      </c>
+      <c r="N18" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O18" s="21">
+        <v>11</v>
+      </c>
+      <c r="P18" s="21">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>22.29</v>
+      </c>
+      <c r="R18" s="21">
         <v>4</v>
       </c>
-      <c r="F18" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" t="s">
-        <v>119</v>
-      </c>
-      <c r="H18" t="s">
-        <v>118</v>
-      </c>
-      <c r="I18">
-        <v>14</v>
-      </c>
-      <c r="J18">
-        <v>9</v>
-      </c>
-      <c r="K18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="S18" s="21">
+        <v>4</v>
+      </c>
+      <c r="T18" s="21">
+        <v>4.6366510391235396</v>
+      </c>
+      <c r="U18" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="F19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="B19" s="5">
+        <v>9.1428571428571406</v>
+      </c>
+      <c r="C19" s="7">
+        <v>9</v>
+      </c>
+      <c r="D19" s="9">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2">
+        <v>44.0833333333333</v>
+      </c>
+      <c r="F19" s="15">
+        <v>9.14</v>
+      </c>
+      <c r="G19" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H19" t="s">
-        <v>121</v>
-      </c>
-      <c r="I19">
+      <c r="H19" s="21">
         <v>23</v>
       </c>
-      <c r="J19">
+      <c r="I19" s="21">
         <v>12</v>
       </c>
-      <c r="K19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="21">
+        <v>31.76</v>
+      </c>
+      <c r="K19" s="21">
+        <v>0.4</v>
+      </c>
+      <c r="L19" s="21">
+        <v>9</v>
+      </c>
+      <c r="M19" s="21">
+        <v>9</v>
+      </c>
+      <c r="N19" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O19" s="21">
+        <v>7</v>
+      </c>
+      <c r="P19" s="21">
+        <v>7</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>21.02</v>
+      </c>
+      <c r="R19" s="21">
+        <v>8</v>
+      </c>
+      <c r="S19" s="21">
+        <v>7</v>
+      </c>
+      <c r="T19" s="21">
+        <v>4.8540370464324996</v>
+      </c>
+      <c r="U19" s="23">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="B20" s="5">
+        <v>6.25</v>
+      </c>
+      <c r="C20" s="7">
+        <v>21.125</v>
+      </c>
+      <c r="D20" s="9">
+        <v>13.5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>10.125</v>
+      </c>
+      <c r="F20" s="15">
+        <v>7.2</v>
+      </c>
+      <c r="G20" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H20" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20">
+      <c r="H20" s="21">
         <v>9</v>
       </c>
-      <c r="J20">
+      <c r="I20" s="21">
         <v>8</v>
       </c>
-      <c r="K20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="21">
+        <v>39.549999999999997</v>
+      </c>
+      <c r="K20" s="21">
+        <v>0.83</v>
+      </c>
+      <c r="L20" s="21">
+        <v>13</v>
+      </c>
+      <c r="M20" s="21">
+        <v>8</v>
+      </c>
+      <c r="N20" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O20" s="21">
+        <v>9</v>
+      </c>
+      <c r="P20" s="21">
+        <v>6</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>25.09</v>
+      </c>
+      <c r="R20" s="21">
+        <v>5</v>
+      </c>
+      <c r="S20" s="21">
+        <v>4</v>
+      </c>
+      <c r="T20" s="21">
+        <v>7.26037693023682</v>
+      </c>
+      <c r="U20" s="23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" t="s">
-        <v>126</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <v>16.6666666666667</v>
+      </c>
+      <c r="D21" s="9">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E21" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="F21" s="15">
+        <v>1</v>
+      </c>
+      <c r="G21" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H21" t="s">
-        <v>77</v>
-      </c>
-      <c r="I21">
+      <c r="H21" s="21">
         <v>6</v>
       </c>
-      <c r="J21">
+      <c r="I21" s="21">
         <v>5</v>
       </c>
-      <c r="K21" t="s">
-        <v>127</v>
+      <c r="J21" s="21">
+        <v>35</v>
+      </c>
+      <c r="K21" s="21">
+        <v>0.88</v>
+      </c>
+      <c r="L21" s="21">
+        <v>10</v>
+      </c>
+      <c r="M21" s="21">
+        <v>6</v>
+      </c>
+      <c r="N21" s="21">
+        <v>11.74</v>
+      </c>
+      <c r="O21" s="21">
+        <v>7</v>
+      </c>
+      <c r="P21" s="21">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>22.05</v>
+      </c>
+      <c r="R21" s="21">
+        <v>1</v>
+      </c>
+      <c r="S21" s="21">
+        <v>1</v>
+      </c>
+      <c r="T21" s="21">
+        <v>0.53260707855224598</v>
+      </c>
+      <c r="U21" s="23">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3279,7 +3864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bergupdate: CGHcall.R: I made all the pipeline parameters available and easy to read & edit. Also I implemented the choice to save the GI results in the current package folder or with all GI results.
</commit_message>
<xml_diff>
--- a/results/GI_all_methods/gi_results_all_methods.xlsx
+++ b/results/GI_all_methods/gi_results_all_methods.xlsx
@@ -1447,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bergupdate: CGHcall generates segtables correctly now
</commit_message>
<xml_diff>
--- a/results/GI_all_methods/gi_results_all_methods.xlsx
+++ b/results/GI_all_methods/gi_results_all_methods.xlsx
@@ -1447,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T22" sqref="T1:U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bergupdate: distribution plot now has correct axes and can even have labels
</commit_message>
<xml_diff>
--- a/results/GI_all_methods/gi_results_all_methods.xlsx
+++ b/results/GI_all_methods/gi_results_all_methods.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="188">
   <si>
     <t>sample</t>
   </si>
@@ -124,9 +124,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>nbAlter_ASCAT</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>0.88</t>
   </si>
   <si>
-    <t>18.05</t>
-  </si>
-  <si>
     <t>21.55</t>
   </si>
   <si>
@@ -244,9 +238,6 @@
     <t>24.1428571428571</t>
   </si>
   <si>
-    <t>18.75</t>
-  </si>
-  <si>
     <t>24.1</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t>35.8</t>
   </si>
   <si>
-    <t>5.33333333333333</t>
-  </si>
-  <si>
     <t>13.5</t>
   </si>
   <si>
@@ -289,9 +277,6 @@
     <t>0.82</t>
   </si>
   <si>
-    <t>60.5</t>
-  </si>
-  <si>
     <t>39.2</t>
   </si>
   <si>
@@ -301,9 +286,6 @@
     <t>33.54</t>
   </si>
   <si>
-    <t>78.125</t>
-  </si>
-  <si>
     <t>105.125</t>
   </si>
   <si>
@@ -343,9 +325,6 @@
     <t>8.33333333333333</t>
   </si>
   <si>
-    <t>4.5</t>
-  </si>
-  <si>
     <t>12.8</t>
   </si>
   <si>
@@ -518,6 +497,93 @@
   </si>
   <si>
     <t>0.51</t>
+  </si>
+  <si>
+    <t>24.76</t>
+  </si>
+  <si>
+    <t>27.1</t>
+  </si>
+  <si>
+    <t>18.7777777777778</t>
+  </si>
+  <si>
+    <t>24.38</t>
+  </si>
+  <si>
+    <t>24.27</t>
+  </si>
+  <si>
+    <t>24.52</t>
+  </si>
+  <si>
+    <t>53.7777777777778</t>
+  </si>
+  <si>
+    <t>24.99</t>
+  </si>
+  <si>
+    <t>17.8181818181818</t>
+  </si>
+  <si>
+    <t>25.01</t>
+  </si>
+  <si>
+    <t>26.01</t>
+  </si>
+  <si>
+    <t>35.5789473684211</t>
+  </si>
+  <si>
+    <t>25.96</t>
+  </si>
+  <si>
+    <t>42.8571428571429</t>
+  </si>
+  <si>
+    <t>26.57</t>
+  </si>
+  <si>
+    <t>36.125</t>
+  </si>
+  <si>
+    <t>33.26</t>
+  </si>
+  <si>
+    <t>55.125</t>
+  </si>
+  <si>
+    <t>27.52</t>
+  </si>
+  <si>
+    <t>82.2857142857143</t>
+  </si>
+  <si>
+    <t>24.37</t>
+  </si>
+  <si>
+    <t>27.36</t>
+  </si>
+  <si>
+    <t>25.66</t>
+  </si>
+  <si>
+    <t>34.14</t>
+  </si>
+  <si>
+    <t>23.34</t>
+  </si>
+  <si>
+    <t>21.125</t>
+  </si>
+  <si>
+    <t>26.95</t>
+  </si>
+  <si>
+    <t>28.76</t>
+  </si>
+  <si>
+    <t>26.14</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1514,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T1:U22"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,13 +1563,13 @@
         <v>32</v>
       </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>37</v>
       </c>
       <c r="K1" t="s">
         <v>25</v>
@@ -1512,7 +1578,7 @@
         <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N1" t="s">
         <v>29</v>
@@ -1521,7 +1587,7 @@
         <v>30</v>
       </c>
       <c r="P1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q1" t="s">
         <v>23</v>
@@ -1530,30 +1596,30 @@
         <v>24</v>
       </c>
       <c r="S1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s">
         <v>38</v>
-      </c>
-      <c r="U1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="5">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="14">
         <v>2</v>
@@ -1568,7 +1634,7 @@
         <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K2" s="4">
         <v>5</v>
@@ -1577,7 +1643,7 @@
         <v>4</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>48</v>
+        <v>159</v>
       </c>
       <c r="N2" s="5">
         <v>4</v>
@@ -1586,7 +1652,7 @@
         <v>2</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="Q2" s="3">
         <v>2</v>
@@ -1595,10 +1661,10 @@
         <v>2</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U2" s="16">
         <v>90</v>
@@ -1609,19 +1675,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>50</v>
+        <v>161</v>
       </c>
       <c r="D3" s="5">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>33</v>
@@ -1633,16 +1699,16 @@
         <v>11</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K3" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L3" s="4">
         <v>9</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>48</v>
+        <v>160</v>
       </c>
       <c r="N3" s="5">
         <v>7</v>
@@ -1651,7 +1717,7 @@
         <v>7</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="Q3" s="3">
         <v>11</v>
@@ -1660,10 +1726,10 @@
         <v>9</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U3" s="16">
         <v>90</v>
@@ -1674,16 +1740,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="4">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F4" s="6">
         <v>15</v>
@@ -1698,16 +1764,16 @@
         <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="4">
         <v>12</v>
       </c>
       <c r="L4" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="N4" s="5">
         <v>12</v>
@@ -1716,7 +1782,7 @@
         <v>10</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="Q4" s="3">
         <v>17</v>
@@ -1725,10 +1791,10 @@
         <v>11</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U4" s="16">
         <v>90</v>
@@ -1742,13 +1808,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="6">
         <v>4</v>
@@ -1763,7 +1829,7 @@
         <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K5" s="4">
         <v>9</v>
@@ -1772,7 +1838,7 @@
         <v>7</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>48</v>
+        <v>163</v>
       </c>
       <c r="N5" s="5">
         <v>1</v>
@@ -1781,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="Q5" s="3">
         <v>4</v>
@@ -1790,10 +1856,10 @@
         <v>4</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="U5" s="17">
         <v>90</v>
@@ -1807,16 +1873,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>50</v>
+        <v>161</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>33</v>
@@ -1828,16 +1894,16 @@
         <v>10</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K6" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L6" s="4">
         <v>9</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>48</v>
+        <v>159</v>
       </c>
       <c r="N6" s="5">
         <v>10</v>
@@ -1846,7 +1912,7 @@
         <v>6</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="Q6" s="3">
         <v>5</v>
@@ -1855,10 +1921,10 @@
         <v>5</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U6" s="17">
         <v>90</v>
@@ -1869,19 +1935,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="4">
-        <v>40</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>33</v>
@@ -1893,16 +1959,16 @@
         <v>10</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K7" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L7" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>48</v>
+        <v>164</v>
       </c>
       <c r="N7" s="5">
         <v>16</v>
@@ -1911,7 +1977,7 @@
         <v>7</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="Q7" s="3">
         <v>6</v>
@@ -1920,10 +1986,10 @@
         <v>5</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="U7" s="17">
         <v>80</v>
@@ -1934,19 +2000,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="F8" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>33</v>
@@ -1958,16 +2024,16 @@
         <v>12</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K8" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L8" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>48</v>
+        <v>166</v>
       </c>
       <c r="N8" s="5">
         <v>11</v>
@@ -1976,7 +2042,7 @@
         <v>9</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q8" s="3">
         <v>13</v>
@@ -1985,7 +2051,7 @@
         <v>7</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="T8" s="1">
         <v>1</v>
@@ -2002,13 +2068,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="D9" s="5">
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F9" s="14">
         <v>1</v>
@@ -2023,16 +2089,16 @@
         <v>6</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="K9" s="4">
+        <v>5</v>
+      </c>
+      <c r="L9" s="4">
         <v>4</v>
       </c>
-      <c r="L9" s="4">
-        <v>3</v>
-      </c>
       <c r="M9" s="4" t="s">
-        <v>48</v>
+        <v>168</v>
       </c>
       <c r="N9" s="5">
         <v>2</v>
@@ -2041,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="Q9" s="3">
         <v>1</v>
@@ -2050,10 +2116,10 @@
         <v>1</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="U9" s="16">
         <v>80</v>
@@ -2067,10 +2133,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E10" s="1">
         <v>5</v>
@@ -2088,16 +2154,16 @@
         <v>5</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K10" s="4">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="L10" s="4">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="N10" s="5">
         <v>5</v>
@@ -2106,7 +2172,7 @@
         <v>3</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="Q10" s="3">
         <v>2</v>
@@ -2115,10 +2181,10 @@
         <v>2</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U10" s="16">
         <v>90</v>
@@ -2131,14 +2197,14 @@
       <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="4">
-        <v>7</v>
+      <c r="C11" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="D11" s="5">
         <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F11" s="14">
         <v>3</v>
@@ -2153,16 +2219,16 @@
         <v>7</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="K11" s="4">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L11" s="4">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="N11" s="5">
         <v>6</v>
@@ -2171,7 +2237,7 @@
         <v>3</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="Q11" s="3">
         <v>2</v>
@@ -2180,10 +2246,10 @@
         <v>2</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="U11" s="16">
         <v>80</v>
@@ -2196,14 +2262,14 @@
       <c r="B12" s="3">
         <v>12</v>
       </c>
-      <c r="C12" s="4">
-        <v>36</v>
+      <c r="C12" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F12" s="14">
         <v>36</v>
@@ -2218,16 +2284,16 @@
         <v>10</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K12" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L12" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>48</v>
+        <v>173</v>
       </c>
       <c r="N12" s="5">
         <v>13</v>
@@ -2236,7 +2302,7 @@
         <v>7</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="Q12" s="3">
         <v>6</v>
@@ -2245,10 +2311,10 @@
         <v>3</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="U12" s="16">
         <v>80</v>
@@ -2262,16 +2328,16 @@
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>33</v>
@@ -2283,16 +2349,16 @@
         <v>7</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="K13" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L13" s="4">
         <v>8</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>48</v>
+        <v>175</v>
       </c>
       <c r="N13" s="5">
         <v>16</v>
@@ -2301,7 +2367,7 @@
         <v>6</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="Q13" s="3">
         <v>0</v>
@@ -2310,10 +2376,10 @@
         <v>0</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U13" s="16">
         <v>90</v>
@@ -2324,16 +2390,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>93</v>
+        <v>178</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F14" s="7">
         <v>60</v>
@@ -2348,16 +2414,16 @@
         <v>8</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="K14" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L14" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>48</v>
+        <v>177</v>
       </c>
       <c r="N14" s="5">
         <v>22</v>
@@ -2366,7 +2432,7 @@
         <v>6</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="Q14" s="3">
         <v>5</v>
@@ -2375,10 +2441,10 @@
         <v>4</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U14" s="16">
         <v>80</v>
@@ -2389,7 +2455,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="4">
         <v>8</v>
@@ -2398,10 +2464,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>33</v>
@@ -2413,7 +2479,7 @@
         <v>9</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="K15" s="4">
         <v>8</v>
@@ -2422,7 +2488,7 @@
         <v>8</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>48</v>
+        <v>179</v>
       </c>
       <c r="N15" s="5">
         <v>0</v>
@@ -2431,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="Q15" s="3">
         <v>11</v>
@@ -2440,10 +2506,10 @@
         <v>9</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="U15" s="17">
         <v>80</v>
@@ -2454,19 +2520,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>33</v>
@@ -2478,7 +2544,7 @@
         <v>13</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K16" s="4">
         <v>13</v>
@@ -2487,7 +2553,7 @@
         <v>7</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="N16" s="5">
         <v>11</v>
@@ -2496,7 +2562,7 @@
         <v>6</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="Q16" s="3">
         <v>8</v>
@@ -2505,10 +2571,10 @@
         <v>6</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="U16" s="16">
         <v>80</v>
@@ -2519,19 +2585,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>33</v>
@@ -2543,16 +2609,16 @@
         <v>8</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="K17" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L17" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>48</v>
+        <v>181</v>
       </c>
       <c r="N17" s="5">
         <v>6</v>
@@ -2561,7 +2627,7 @@
         <v>5</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="Q17" s="3">
         <v>8</v>
@@ -2570,10 +2636,10 @@
         <v>6</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="U17" s="16">
         <v>90</v>
@@ -2584,19 +2650,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>33</v>
@@ -2608,16 +2674,16 @@
         <v>17</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="K18" s="4">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L18" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="N18" s="5">
         <v>5</v>
@@ -2626,7 +2692,7 @@
         <v>3</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="Q18" s="3">
         <v>5</v>
@@ -2635,7 +2701,7 @@
         <v>3</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="T18" s="1">
         <v>1</v>
@@ -2652,19 +2718,19 @@
         <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="D19" s="5">
         <v>24</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H19" s="1">
         <v>14</v>
@@ -2673,16 +2739,16 @@
         <v>9</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="K19" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L19" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>48</v>
+        <v>183</v>
       </c>
       <c r="N19" s="5">
         <v>12</v>
@@ -2691,7 +2757,7 @@
         <v>6</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="Q19" s="3">
         <v>4</v>
@@ -2700,10 +2766,10 @@
         <v>4</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="U19" s="17">
         <v>100</v>
@@ -2714,19 +2780,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C20" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="5">
         <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>33</v>
@@ -2738,16 +2804,16 @@
         <v>12</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="K20" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L20" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>48</v>
+        <v>185</v>
       </c>
       <c r="N20" s="5">
         <v>7</v>
@@ -2756,7 +2822,7 @@
         <v>7</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="Q20" s="3">
         <v>8</v>
@@ -2765,10 +2831,10 @@
         <v>7</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="U20" s="17">
         <v>95</v>
@@ -2779,19 +2845,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>103</v>
+        <v>184</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>33</v>
@@ -2803,16 +2869,16 @@
         <v>8</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="K21" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L21" s="4">
         <v>8</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="N21" s="5">
         <v>9</v>
@@ -2821,7 +2887,7 @@
         <v>6</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="Q21" s="3">
         <v>5</v>
@@ -2830,10 +2896,10 @@
         <v>4</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U21" s="17">
         <v>80</v>
@@ -2847,13 +2913,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F22" s="15">
         <v>1</v>
@@ -2868,7 +2934,7 @@
         <v>5</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K22" s="4">
         <v>10</v>
@@ -2877,7 +2943,7 @@
         <v>6</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>48</v>
+        <v>187</v>
       </c>
       <c r="N22" s="5">
         <v>7</v>
@@ -2886,7 +2952,7 @@
         <v>5</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="Q22" s="3">
         <v>1</v>
@@ -2895,10 +2961,10 @@
         <v>1</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U22" s="17">
         <v>80</v>
@@ -2912,7 +2978,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
@@ -3406,11 +3472,6 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bergupdate: about to change CGHcall.R's plotSegTable() fx so I backup
</commit_message>
<xml_diff>
--- a/results/GI_all_methods/gi_results_all_methods.xlsx
+++ b/results/GI_all_methods/gi_results_all_methods.xlsx
@@ -14,13 +14,14 @@
   <sheets>
     <sheet name="new_gi_all_methods" sheetId="3" r:id="rId1"/>
     <sheet name="to_export" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="244">
   <si>
     <t>sample</t>
   </si>
@@ -157,9 +158,6 @@
     <t>11.1111111111111</t>
   </si>
   <si>
-    <t>97.55</t>
-  </si>
-  <si>
     <t>0.88</t>
   </si>
   <si>
@@ -584,13 +582,184 @@
   </si>
   <si>
     <t>26.14</t>
+  </si>
+  <si>
+    <t>37.06</t>
+  </si>
+  <si>
+    <t>Chromosome</t>
+  </si>
+  <si>
+    <t>Total base pairs</t>
+  </si>
+  <si>
+    <t>247,199,719</t>
+  </si>
+  <si>
+    <t>242,751,149</t>
+  </si>
+  <si>
+    <t>199,446,827</t>
+  </si>
+  <si>
+    <t>191,263,063</t>
+  </si>
+  <si>
+    <t>180,837,866</t>
+  </si>
+  <si>
+    <t>170,896,993</t>
+  </si>
+  <si>
+    <t>158,821,424</t>
+  </si>
+  <si>
+    <t>146,274,826</t>
+  </si>
+  <si>
+    <t>140,442,298</t>
+  </si>
+  <si>
+    <t>135,374,737</t>
+  </si>
+  <si>
+    <t>134,452,384</t>
+  </si>
+  <si>
+    <t>132,289,534</t>
+  </si>
+  <si>
+    <t>114,127,980</t>
+  </si>
+  <si>
+    <t>106,360,585</t>
+  </si>
+  <si>
+    <t>100,338,915</t>
+  </si>
+  <si>
+    <t>88,822,254</t>
+  </si>
+  <si>
+    <t>78,654,742</t>
+  </si>
+  <si>
+    <t>76,117,153</t>
+  </si>
+  <si>
+    <t>63,806,651</t>
+  </si>
+  <si>
+    <t>62,435,965</t>
+  </si>
+  <si>
+    <t>46,944,323</t>
+  </si>
+  <si>
+    <t>49,528,953</t>
+  </si>
+  <si>
+    <t>154,913,754</t>
+  </si>
+  <si>
+    <t>57,741,652</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>8.00</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>9.00</t>
+  </si>
+  <si>
+    <t>5.00</t>
+  </si>
+  <si>
+    <t>4.00</t>
+  </si>
+  <si>
+    <t>7.00</t>
+  </si>
+  <si>
+    <t>16.00</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>13.00</t>
+  </si>
+  <si>
+    <t>18.00</t>
+  </si>
+  <si>
+    <t>22.5</t>
+  </si>
+  <si>
+    <t>39.00</t>
+  </si>
+  <si>
+    <t>22.00</t>
+  </si>
+  <si>
+    <t>12.00</t>
+  </si>
+  <si>
+    <t>17.00</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>25.00</t>
+  </si>
+  <si>
+    <t>14.00</t>
+  </si>
+  <si>
+    <t>26.00</t>
+  </si>
+  <si>
+    <t>19.00</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>30.00</t>
+  </si>
+  <si>
+    <t>21.00</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>29.00</t>
+  </si>
+  <si>
+    <t>24.00</t>
+  </si>
+  <si>
+    <t>82.00</t>
+  </si>
+  <si>
+    <t>23.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,6 +897,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1106,7 +1283,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1149,8 +1326,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1181,8 +1359,23 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1213,6 +1406,7 @@
     <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Lien hypertexte" xfId="42" builtinId="8"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
@@ -1514,7 +1708,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,14 +1803,14 @@
       <c r="A2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="3">
-        <v>2</v>
+      <c r="B2" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="5">
-        <v>8</v>
+      <c r="D2" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>44</v>
@@ -1627,44 +1821,44 @@
       <c r="G2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="1">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1">
-        <v>9</v>
+      <c r="H2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="K2" s="4">
-        <v>5</v>
-      </c>
-      <c r="L2" s="4">
-        <v>4</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="N2" s="5">
-        <v>4</v>
-      </c>
-      <c r="O2" s="5">
-        <v>2</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>2</v>
-      </c>
-      <c r="R2" s="3">
-        <v>2</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="U2" s="16">
         <v>90</v>
@@ -1675,61 +1869,61 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3" s="5">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1">
-        <v>11</v>
+      <c r="H3" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="K3" s="4">
-        <v>13</v>
-      </c>
-      <c r="L3" s="4">
-        <v>9</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="N3" s="5">
-        <v>7</v>
-      </c>
-      <c r="O3" s="5">
-        <v>7</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>11</v>
-      </c>
-      <c r="R3" s="3">
-        <v>9</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="U3" s="16">
         <v>90</v>
@@ -1740,61 +1934,61 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="4">
-        <v>18</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="6">
-        <v>22.5</v>
+      <c r="F4" s="6" t="s">
+        <v>225</v>
       </c>
       <c r="G4" s="6">
         <v>15</v>
       </c>
-      <c r="H4" s="1">
-        <v>39</v>
-      </c>
-      <c r="I4" s="1">
-        <v>22</v>
+      <c r="H4" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="K4" s="4">
-        <v>12</v>
-      </c>
-      <c r="L4" s="4">
-        <v>8</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="N4" s="5">
-        <v>12</v>
-      </c>
-      <c r="O4" s="5">
-        <v>10</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>17</v>
-      </c>
-      <c r="R4" s="3">
-        <v>11</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="U4" s="16">
         <v>90</v>
@@ -1804,17 +1998,17 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>4</v>
+      <c r="B5" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="F5" s="6">
         <v>4</v>
@@ -1822,44 +2016,44 @@
       <c r="G5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="1">
-        <v>9</v>
-      </c>
-      <c r="I5" s="1">
-        <v>8</v>
+      <c r="H5" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="K5" s="4">
-        <v>9</v>
-      </c>
-      <c r="L5" s="4">
-        <v>7</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="N5" s="5">
-        <v>1</v>
-      </c>
-      <c r="O5" s="5">
-        <v>1</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>4</v>
-      </c>
-      <c r="R5" s="3">
-        <v>4</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="U5" s="17">
         <v>90</v>
@@ -1869,62 +2063,62 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>5</v>
+      <c r="B6" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="1">
-        <v>16</v>
-      </c>
-      <c r="I6" s="1">
-        <v>10</v>
+      <c r="H6" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="K6" s="4">
-        <v>13</v>
-      </c>
-      <c r="L6" s="4">
-        <v>9</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="N6" s="5">
-        <v>10</v>
-      </c>
-      <c r="O6" s="5">
-        <v>6</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>5</v>
-      </c>
-      <c r="R6" s="3">
-        <v>5</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="U6" s="17">
         <v>90</v>
@@ -1935,61 +2129,61 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="1">
-        <v>25</v>
-      </c>
-      <c r="I7" s="1">
-        <v>10</v>
+      <c r="H7" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="K7" s="4">
-        <v>22</v>
-      </c>
-      <c r="L7" s="4">
-        <v>9</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="N7" s="5">
-        <v>16</v>
-      </c>
-      <c r="O7" s="5">
-        <v>7</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>6</v>
-      </c>
-      <c r="R7" s="3">
-        <v>5</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="U7" s="17">
         <v>80</v>
@@ -2000,61 +2194,61 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>72</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="1">
-        <v>16</v>
-      </c>
-      <c r="I8" s="1">
-        <v>12</v>
+      <c r="H8" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" s="4">
-        <v>14</v>
-      </c>
-      <c r="L8" s="4">
-        <v>11</v>
+        <v>73</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>222</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="N8" s="5">
-        <v>11</v>
-      </c>
-      <c r="O8" s="5">
-        <v>9</v>
+        <v>165</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>13</v>
-      </c>
-      <c r="R8" s="3">
-        <v>7</v>
+        <v>46</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="T8" s="1">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="U8" s="17">
         <v>90</v>
@@ -2064,17 +2258,17 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>1</v>
+      <c r="B9" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="5">
-        <v>4</v>
+      <c r="D9" s="5" t="s">
+        <v>219</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="14">
         <v>1</v>
@@ -2082,44 +2276,44 @@
       <c r="G9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="1">
-        <v>9</v>
-      </c>
-      <c r="I9" s="1">
-        <v>6</v>
+      <c r="H9" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="K9" s="4">
-        <v>5</v>
-      </c>
-      <c r="L9" s="4">
-        <v>4</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="N9" s="5">
-        <v>2</v>
-      </c>
-      <c r="O9" s="5">
-        <v>1</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>1</v>
-      </c>
-      <c r="R9" s="3">
-        <v>1</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="U9" s="16">
         <v>80</v>
@@ -2129,17 +2323,17 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
-        <v>2</v>
+      <c r="B10" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5</v>
+        <v>99</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="F10" s="14">
         <v>2</v>
@@ -2147,44 +2341,44 @@
       <c r="G10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="1">
-        <v>5</v>
-      </c>
-      <c r="I10" s="1">
-        <v>5</v>
+      <c r="H10" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K10" s="4">
-        <v>26</v>
-      </c>
-      <c r="L10" s="4">
-        <v>19</v>
+        <v>77</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>235</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="N10" s="5">
-        <v>5</v>
-      </c>
-      <c r="O10" s="5">
-        <v>3</v>
+        <v>168</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="P10" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="S10" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="Q10" s="3">
-        <v>2</v>
-      </c>
-      <c r="R10" s="3">
-        <v>2</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="T10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U10" s="16">
         <v>90</v>
@@ -2194,17 +2388,17 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>2</v>
+      <c r="B11" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="5">
-        <v>12</v>
+        <v>171</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="14">
         <v>3</v>
@@ -2212,44 +2406,44 @@
       <c r="G11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="1">
-        <v>8</v>
-      </c>
-      <c r="I11" s="1">
-        <v>7</v>
+      <c r="H11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="J11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="K11" s="4">
-        <v>30</v>
-      </c>
-      <c r="L11" s="4">
-        <v>21</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="N11" s="5">
-        <v>6</v>
-      </c>
-      <c r="O11" s="5">
-        <v>3</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>2</v>
-      </c>
-      <c r="R11" s="3">
-        <v>2</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="U11" s="16">
         <v>80</v>
@@ -2259,17 +2453,17 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
-        <v>12</v>
+      <c r="B12" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" s="14">
         <v>36</v>
@@ -2277,44 +2471,44 @@
       <c r="G12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="1">
-        <v>18</v>
-      </c>
-      <c r="I12" s="1">
-        <v>10</v>
+      <c r="H12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="K12" s="4">
-        <v>17</v>
-      </c>
-      <c r="L12" s="4">
-        <v>8</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="N12" s="5">
-        <v>13</v>
-      </c>
-      <c r="O12" s="5">
-        <v>7</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>6</v>
-      </c>
-      <c r="R12" s="3">
-        <v>3</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="U12" s="16">
         <v>80</v>
@@ -2324,62 +2518,62 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>0</v>
+      <c r="B13" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="1">
-        <v>18</v>
-      </c>
-      <c r="I13" s="1">
-        <v>7</v>
+      <c r="H13" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K13" s="4">
-        <v>21</v>
-      </c>
-      <c r="L13" s="4">
-        <v>8</v>
+        <v>86</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="N13" s="5">
-        <v>16</v>
-      </c>
-      <c r="O13" s="5">
-        <v>6</v>
+        <v>174</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="P13" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="S13" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="Q13" s="3">
-        <v>0</v>
-      </c>
-      <c r="R13" s="3">
-        <v>0</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="T13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U13" s="16">
         <v>90</v>
@@ -2393,13 +2587,13 @@
         <v>43</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" s="7">
         <v>60</v>
@@ -2407,44 +2601,44 @@
       <c r="G14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="1">
-        <v>29</v>
-      </c>
-      <c r="I14" s="1">
-        <v>8</v>
+      <c r="H14" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14" s="4">
-        <v>24</v>
-      </c>
-      <c r="L14" s="4">
-        <v>7</v>
+        <v>88</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>220</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="N14" s="5">
-        <v>22</v>
-      </c>
-      <c r="O14" s="5">
-        <v>6</v>
+        <v>176</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="P14" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="S14" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="Q14" s="3">
-        <v>5</v>
-      </c>
-      <c r="R14" s="3">
-        <v>4</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="T14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U14" s="16">
         <v>80</v>
@@ -2455,61 +2649,61 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="C15" s="4">
-        <v>8</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="1">
-        <v>11</v>
-      </c>
-      <c r="I15" s="1">
-        <v>9</v>
+      <c r="H15" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="K15" s="4">
-        <v>8</v>
-      </c>
-      <c r="L15" s="4">
-        <v>8</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-      <c r="O15" s="5">
-        <v>0</v>
-      </c>
-      <c r="P15" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>11</v>
-      </c>
-      <c r="R15" s="3">
-        <v>9</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="U15" s="17">
         <v>80</v>
@@ -2520,61 +2714,61 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>92</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>93</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="1">
-        <v>17</v>
-      </c>
-      <c r="I16" s="1">
-        <v>13</v>
+      <c r="H16" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="J16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="T16" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="K16" s="4">
-        <v>13</v>
-      </c>
-      <c r="L16" s="4">
-        <v>7</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="N16" s="5">
-        <v>11</v>
-      </c>
-      <c r="O16" s="5">
-        <v>6</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>8</v>
-      </c>
-      <c r="R16" s="3">
-        <v>6</v>
-      </c>
-      <c r="S16" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="U16" s="16">
         <v>80</v>
@@ -2585,61 +2779,61 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>92</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>93</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="1">
-        <v>11</v>
-      </c>
-      <c r="I17" s="1">
-        <v>8</v>
+      <c r="H17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="T17" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="K17" s="4">
-        <v>9</v>
-      </c>
-      <c r="L17" s="4">
-        <v>6</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="N17" s="5">
-        <v>6</v>
-      </c>
-      <c r="O17" s="5">
-        <v>5</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>8</v>
-      </c>
-      <c r="R17" s="3">
-        <v>6</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="U17" s="16">
         <v>90</v>
@@ -2650,61 +2844,61 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>101</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="1">
-        <v>82</v>
-      </c>
-      <c r="I18" s="1">
-        <v>17</v>
+      <c r="H18" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K18" s="4">
-        <v>10</v>
-      </c>
-      <c r="L18" s="4">
-        <v>9</v>
+        <v>102</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="N18" s="5">
-        <v>5</v>
-      </c>
-      <c r="O18" s="5">
-        <v>3</v>
+        <v>181</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="P18" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="S18" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="Q18" s="3">
-        <v>5</v>
-      </c>
-      <c r="R18" s="3">
-        <v>3</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="T18" s="1">
-        <v>1</v>
+      <c r="T18" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="U18" s="16">
         <v>80</v>
@@ -2714,62 +2908,62 @@
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
-        <v>4</v>
+      <c r="B19" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D19" s="5">
-        <v>24</v>
+        <v>183</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="15" t="s">
+      <c r="H19" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H19" s="1">
-        <v>14</v>
-      </c>
-      <c r="I19" s="1">
-        <v>9</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="T19" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="K19" s="4">
-        <v>13</v>
-      </c>
-      <c r="L19" s="4">
-        <v>8</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="N19" s="5">
-        <v>12</v>
-      </c>
-      <c r="O19" s="5">
-        <v>6</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>4</v>
-      </c>
-      <c r="R19" s="3">
-        <v>4</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="U19" s="17">
         <v>100</v>
@@ -2780,61 +2974,61 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="4">
-        <v>9</v>
-      </c>
-      <c r="D20" s="5">
-        <v>7</v>
+        <v>78</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>220</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="1">
-        <v>23</v>
-      </c>
-      <c r="I20" s="1">
-        <v>12</v>
+      <c r="H20" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K20" s="4">
-        <v>9</v>
-      </c>
-      <c r="L20" s="4">
-        <v>9</v>
+        <v>86</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="N20" s="5">
-        <v>7</v>
-      </c>
-      <c r="O20" s="5">
-        <v>7</v>
+        <v>184</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>220</v>
       </c>
       <c r="P20" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="S20" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="Q20" s="3">
-        <v>8</v>
-      </c>
-      <c r="R20" s="3">
-        <v>7</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="T20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U20" s="17">
         <v>95</v>
@@ -2848,58 +3042,58 @@
         <v>43</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="1">
-        <v>9</v>
-      </c>
-      <c r="I21" s="1">
-        <v>8</v>
+      <c r="H21" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="K21" s="4">
-        <v>13</v>
-      </c>
-      <c r="L21" s="4">
-        <v>8</v>
+        <v>109</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="N21" s="5">
-        <v>9</v>
-      </c>
-      <c r="O21" s="5">
-        <v>6</v>
+        <v>185</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="P21" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="S21" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q21" s="3">
-        <v>5</v>
-      </c>
-      <c r="R21" s="3">
-        <v>4</v>
-      </c>
-      <c r="S21" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="T21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U21" s="17">
         <v>80</v>
@@ -2909,17 +3103,17 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
-        <v>1</v>
+      <c r="B22" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" s="15">
         <v>1</v>
@@ -2927,44 +3121,44 @@
       <c r="G22" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H22" s="1">
-        <v>6</v>
-      </c>
-      <c r="I22" s="1">
-        <v>5</v>
+      <c r="H22" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K22" s="4">
-        <v>10</v>
-      </c>
-      <c r="L22" s="4">
-        <v>6</v>
+        <v>111</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="N22" s="5">
-        <v>7</v>
-      </c>
-      <c r="O22" s="5">
-        <v>5</v>
+        <v>186</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="P22" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="S22" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="Q22" s="3">
-        <v>1</v>
-      </c>
-      <c r="R22" s="3">
-        <v>1</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="T22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U22" s="17">
         <v>80</v>
@@ -3475,4 +3669,278 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="20"/>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="20"/>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="20"/>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="20"/>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="20"/>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="20"/>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="20"/>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="20"/>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="20"/>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="20"/>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="20"/>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="20"/>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="20"/>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="20"/>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="20"/>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="20"/>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="20"/>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="20"/>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="20"/>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="20"/>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="20"/>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="20"/>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="20"/>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>